<commit_message>
fix: enhance PDF generation process for improved performance
</commit_message>
<xml_diff>
--- a/templates/summaryTemplate.xlsx
+++ b/templates/summaryTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="498" documentId="13_ncr:1_{C26209B1-5C57-41BE-91B5-396332C4B2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B49339EB-DA51-4F68-8419-C1027F5B3B7F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5680F9A-5EDA-46D1-9707-C7F0D96C43A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,33 +621,33 @@
   </sheetPr>
   <dimension ref="A2:M9"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="66" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.26953125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7265625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
     </row>
-    <row r="4" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -662,7 +662,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -693,7 +693,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -734,7 +734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -749,7 +749,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -764,7 +764,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -801,20 +801,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDD6085FA6890649A3A665E7D5B8DC26" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c854d55ac5d19a7389dbe528e0729ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="50af9aba-9198-462f-98f3-1e3a097082a8" xmlns:ns3="da240321-5779-415a-a19b-d3870c14c12d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1531ee9ef5d57e80513a6cf4b2fa5b5" ns2:_="" ns3:_="">
     <xsd:import namespace="50af9aba-9198-462f-98f3-1e3a097082a8"/>
@@ -1021,6 +1007,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1033,22 +1033,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E648C8C-6C17-4FFD-8B22-CF85884EDF45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1067,6 +1051,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547DB070-782C-45D3-9B06-6FB235F7BBFE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat: enable conditional row insertion in ACC_Smart_Forms based on data presence
</commit_message>
<xml_diff>
--- a/templates/summaryTemplate.xlsx
+++ b/templates/summaryTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5680F9A-5EDA-46D1-9707-C7F0D96C43A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742F335E-A2D8-4CD4-B9AC-EB6DD42D19D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$M$9</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -623,7 +624,7 @@
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -801,6 +802,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDD6085FA6890649A3A665E7D5B8DC26" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c854d55ac5d19a7389dbe528e0729ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="50af9aba-9198-462f-98f3-1e3a097082a8" xmlns:ns3="da240321-5779-415a-a19b-d3870c14c12d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1531ee9ef5d57e80513a6cf4b2fa5b5" ns2:_="" ns3:_="">
     <xsd:import namespace="50af9aba-9198-462f-98f3-1e3a097082a8"/>
@@ -1007,20 +1022,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1033,6 +1034,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E648C8C-6C17-4FFD-8B22-CF85884EDF45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1051,22 +1068,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547DB070-782C-45D3-9B06-6FB235F7BBFE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat: improve error handling in PDF generation process to enhance stability
</commit_message>
<xml_diff>
--- a/templates/summaryTemplate.xlsx
+++ b/templates/summaryTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742F335E-A2D8-4CD4-B9AC-EB6DD42D19D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440BF5B3-DE0E-467F-A4EA-913F07FB8459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$M$9</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -217,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -254,9 +254,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,7 +621,7 @@
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -766,26 +763,25 @@
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
       <c r="L9" s="5"/>
       <c r="M9" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:M9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="A2"/>
-    <mergeCell ref="A9:K9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
@@ -802,20 +798,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDD6085FA6890649A3A665E7D5B8DC26" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c854d55ac5d19a7389dbe528e0729ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="50af9aba-9198-462f-98f3-1e3a097082a8" xmlns:ns3="da240321-5779-415a-a19b-d3870c14c12d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1531ee9ef5d57e80513a6cf4b2fa5b5" ns2:_="" ns3:_="">
     <xsd:import namespace="50af9aba-9198-462f-98f3-1e3a097082a8"/>
@@ -1022,6 +1004,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1034,22 +1030,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E648C8C-6C17-4FFD-8B22-CF85884EDF45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1068,6 +1048,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547DB070-782C-45D3-9B06-6FB235F7BBFE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat: optimize PDF generation performance by reducing processing time and memory usage
</commit_message>
<xml_diff>
--- a/templates/summaryTemplate.xlsx
+++ b/templates/summaryTemplate.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440BF5B3-DE0E-467F-A4EA-913F07FB8459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="498" documentId="13_ncr:1_{C26209B1-5C57-41BE-91B5-396332C4B2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B49339EB-DA51-4F68-8419-C1027F5B3B7F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$M$9</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -217,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -254,6 +253,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,33 +621,33 @@
   </sheetPr>
   <dimension ref="A2:M9"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.26953125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" style="1" customWidth="1"/>
     <col min="14" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
     </row>
-    <row r="4" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -660,7 +662,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -691,7 +693,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -732,7 +734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -747,7 +749,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -762,26 +764,27 @@
       <c r="L8" s="8"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="5"/>
       <c r="M9" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:M9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="A2"/>
+    <mergeCell ref="A9:K9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
@@ -798,6 +801,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDD6085FA6890649A3A665E7D5B8DC26" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c854d55ac5d19a7389dbe528e0729ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="50af9aba-9198-462f-98f3-1e3a097082a8" xmlns:ns3="da240321-5779-415a-a19b-d3870c14c12d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1531ee9ef5d57e80513a6cf4b2fa5b5" ns2:_="" ns3:_="">
     <xsd:import namespace="50af9aba-9198-462f-98f3-1e3a097082a8"/>
@@ -1004,20 +1021,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1030,6 +1033,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E648C8C-6C17-4FFD-8B22-CF85884EDF45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1048,22 +1067,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547DB070-782C-45D3-9B06-6FB235F7BBFE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat: streamline PDF generation workflow by implementing batch processing for multiple files
</commit_message>
<xml_diff>
--- a/templates/summaryTemplate.xlsx
+++ b/templates/summaryTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="498" documentId="13_ncr:1_{C26209B1-5C57-41BE-91B5-396332C4B2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B49339EB-DA51-4F68-8419-C1027F5B3B7F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CA749F-7521-4C11-90EF-3EFD7D4DEFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -253,9 +253,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,31 +620,31 @@
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="66" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.26953125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7265625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
     </row>
-    <row r="4" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -662,7 +659,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -693,7 +690,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -734,7 +731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -749,7 +746,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -764,27 +761,26 @@
       <c r="L8" s="8"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
+    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
       <c r="L9" s="5"/>
       <c r="M9" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:M9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="A2"/>
-    <mergeCell ref="A9:K9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
@@ -801,20 +797,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDD6085FA6890649A3A665E7D5B8DC26" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c854d55ac5d19a7389dbe528e0729ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="50af9aba-9198-462f-98f3-1e3a097082a8" xmlns:ns3="da240321-5779-415a-a19b-d3870c14c12d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1531ee9ef5d57e80513a6cf4b2fa5b5" ns2:_="" ns3:_="">
     <xsd:import namespace="50af9aba-9198-462f-98f3-1e3a097082a8"/>
@@ -1021,6 +1003,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1033,22 +1029,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E648C8C-6C17-4FFD-8B22-CF85884EDF45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1067,6 +1047,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547DB070-782C-45D3-9B06-6FB235F7BBFE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
feat: update refresh token in refresh_token.txt
</commit_message>
<xml_diff>
--- a/templates/summaryTemplate.xlsx
+++ b/templates/summaryTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CA749F-7521-4C11-90EF-3EFD7D4DEFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22349A1E-7BE2-4510-9A5F-A01DAA5E05CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -212,11 +212,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,9 +258,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,9 +628,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:M9"/>
+  <dimension ref="A2:U9"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9:K9"/>
     </sheetView>
@@ -641,25 +653,36 @@
     <col min="14" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
     </row>
-    <row r="4" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
+    <row r="4" spans="1:21" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="13" t="str">
+        <f ca="1">" ملخص بيان اعمال  ( المعدات - رفع المخلفات ) عن الفترة من " &amp; "01/" &amp; TEXT(TODAY(),"mm/yyyy") &amp; " حتي " &amp; DAY(EOMONTH(TODAY(),0)) &amp; "/" &amp; TEXT(TODAY(),"mm/yyyy") &amp; " المشروع: " &amp; A7</f>
+        <v xml:space="preserve"> ملخص بيان اعمال  ( المعدات - رفع المخلفات ) عن الفترة من 01/02/2025 حتي 28/02/2025 المشروع: </v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -690,7 +713,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -731,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -746,7 +769,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -761,7 +784,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -779,8 +802,8 @@
   </sheetData>
   <autoFilter ref="A6:M9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="2">
+    <mergeCell ref="A2"/>
     <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
@@ -797,6 +820,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EDD6085FA6890649A3A665E7D5B8DC26" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c854d55ac5d19a7389dbe528e0729ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="50af9aba-9198-462f-98f3-1e3a097082a8" xmlns:ns3="da240321-5779-415a-a19b-d3870c14c12d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1531ee9ef5d57e80513a6cf4b2fa5b5" ns2:_="" ns3:_="">
     <xsd:import namespace="50af9aba-9198-462f-98f3-1e3a097082a8"/>
@@ -1003,21 +1031,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c77a068b-8bd6-40cc-a27e-cb2ff04b6c5f" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="50af9aba-9198-462f-98f3-1e3a097082a8">
@@ -1028,7 +1042,24 @@
 </p:properties>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E648C8C-6C17-4FFD-8B22-CF85884EDF45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1047,23 +1078,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB718D1-6387-40C0-B3D9-84AAD762CA94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547DB070-782C-45D3-9B06-6FB235F7BBFE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1072,4 +1087,12 @@
     <ds:schemaRef ds:uri="da240321-5779-415a-a19b-d3870c14c12d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E57C66-7E7C-490C-BE43-371DC5D06E3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>